<commit_message>
Removed raise comments from 'history'
</commit_message>
<xml_diff>
--- a/metadata/flux_metadata_level1_15min_June2022.xlsx
+++ b/metadata/flux_metadata_level1_15min_June2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8984E80D-157D-8442-942C-DD594C307B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031DBEDA-6798-8E4C-9329-D9475272159A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -264,10 +264,10 @@
     <t>timeSeries</t>
   </si>
   <si>
-    <t>Data collection start: 2019-06-01T00:00:00. Instruments raised by ~ 1 m on 01 July 2021  (see comment for heights)</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 Hz sampling rate on both licor and sonic. Runs 15 mins in length. Run time stamp: start of run. </t>
+  </si>
+  <si>
+    <t>Data collection start: 2019-06-01T00:00:00.</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1034,7 +1034,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1042,7 +1042,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>